<commit_message>
queries for two approaches: top1, top5, top10
</commit_message>
<xml_diff>
--- a/data/testQueriesEvaluation.xlsx
+++ b/data/testQueriesEvaluation.xlsx
@@ -10,6 +10,8 @@
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Evaluations" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Groups" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t xml:space="preserve">Queries</t>
   </si>
@@ -32,25 +34,7 @@
     <t xml:space="preserve">Solution A</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Solution</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> B</t>
-    </r>
+    <t xml:space="preserve">Solution B</t>
   </si>
   <si>
     <t xml:space="preserve">Mark the relevance of suggested code Snippets</t>
@@ -135,6 +119,12 @@
   </si>
   <si>
     <t xml:space="preserve">Using Images in an Applet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
   </si>
 </sst>
 </file>
@@ -144,7 +134,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -172,12 +162,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -236,7 +220,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -258,10 +242,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -302,7 +282,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData/>
@@ -324,7 +304,7 @@
   <dimension ref="A1:AMJ27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -332,7 +312,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.48"/>
@@ -352,31 +332,31 @@
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="8"/>
-      <c r="C2" s="9" t="s">
+    <row r="2" s="6" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="7"/>
+      <c r="C2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="AMJ2" s="0"/>
@@ -422,8 +402,8 @@
         <v>11</v>
       </c>
       <c r="B7" s="1" t="str">
-        <f aca="false">HYPERLINK("https://kodejava.org/category/java/core-api/page/33/")</f>
-        <v>https://kodejava.org/category/java/core-api/page/33/</v>
+        <f aca="false">HYPERLINK("$Instructions.P14")</f>
+        <v>$Instructions.P14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -619,4 +599,93 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A12"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="60.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
just before replication package
</commit_message>
<xml_diff>
--- a/data/testQueriesEvaluation.xlsx
+++ b/data/testQueriesEvaluation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
   <si>
     <t xml:space="preserve">Queries</t>
   </si>
@@ -124,7 +124,49 @@
     <t xml:space="preserve">A</t>
   </si>
   <si>
+    <t xml:space="preserve">Guilherme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eduardo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carlos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enviado esperando</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Victor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fernanda</t>
+  </si>
+  <si>
     <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rogerio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nao enviado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adriano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hammid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guilherme Friends</t>
   </si>
 </sst>
 </file>
@@ -303,8 +345,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -606,16 +648,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="60.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.17"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -627,30 +671,187 @@
       <c r="A2" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="B2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="B3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>21</v>
       </c>
+      <c r="B4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="B5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>22</v>
       </c>
+      <c r="B6" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>